<commit_message>
traces leds complete (for now)
</commit_message>
<xml_diff>
--- a/Angles.xlsx
+++ b/Angles.xlsx
@@ -478,7 +478,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1018,207 +1018,207 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="13">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B26" s="13">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13">
         <f t="shared" si="1"/>
-        <v>56.180339887498945</v>
+        <v>50</v>
       </c>
       <c r="E26" s="13">
         <f t="shared" si="2"/>
-        <v>69.021130325903073</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="13">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B27" s="13">
         <f>B26+30</f>
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13">
         <f t="shared" si="1"/>
-        <v>64.86289650954788</v>
+        <v>58.5</v>
       </c>
       <c r="E27" s="13">
         <f t="shared" si="2"/>
-        <v>63.382612127177168</v>
+        <v>64.722431864335462</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="13">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B28">
         <f t="shared" ref="B28:B32" si="5">B27+30</f>
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D28">
         <f t="shared" ref="D28:D32" si="6">50+A28*SIN(RADIANS(B28))</f>
-        <v>69.562952014676114</v>
+        <v>64.722431864335462</v>
       </c>
       <c r="E28">
         <f t="shared" ref="E28:E32" si="7">50+A28*COS(RADIANS(B28))</f>
-        <v>54.158233816355192</v>
+        <v>58.5</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="13">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B29">
         <f t="shared" si="5"/>
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="D29">
         <f t="shared" si="6"/>
-        <v>69.021130325903073</v>
+        <v>67</v>
       </c>
       <c r="E29">
         <f t="shared" si="7"/>
-        <v>43.819660112501055</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="13">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B30">
         <f t="shared" si="5"/>
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="D30">
         <f t="shared" si="6"/>
-        <v>63.382612127177168</v>
+        <v>64.722431864335462</v>
       </c>
       <c r="E30">
         <f t="shared" si="7"/>
-        <v>35.13710349045212</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="13">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B31">
         <f t="shared" si="5"/>
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="D31">
         <f t="shared" si="6"/>
-        <v>54.158233816355185</v>
+        <v>58.5</v>
       </c>
       <c r="E31">
         <f t="shared" si="7"/>
-        <v>30.437047985323886</v>
+        <v>35.277568135664538</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="13">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B32">
         <f t="shared" si="5"/>
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D32">
         <f t="shared" si="6"/>
-        <v>43.819660112501055</v>
+        <v>50</v>
       </c>
       <c r="E32">
         <f t="shared" si="7"/>
-        <v>30.978869674096927</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="13">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B33">
         <f t="shared" ref="B33:B37" si="8">B32+30</f>
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="D33">
         <f t="shared" ref="D33:D37" si="9">50+A33*SIN(RADIANS(B33))</f>
-        <v>35.137103490452112</v>
+        <v>41.5</v>
       </c>
       <c r="E33">
         <f t="shared" ref="E33:E37" si="10">50+A33*COS(RADIANS(B33))</f>
-        <v>36.617387872822839</v>
+        <v>35.277568135664545</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="13">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B34">
         <f t="shared" si="8"/>
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="D34">
         <f t="shared" si="9"/>
-        <v>30.43704798532389</v>
+        <v>35.277568135664552</v>
       </c>
       <c r="E34">
         <f t="shared" si="10"/>
-        <v>45.841766183644808</v>
+        <v>41.499999999999993</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="13">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B35">
         <f t="shared" si="8"/>
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="D35">
         <f t="shared" si="9"/>
-        <v>30.978869674096927</v>
+        <v>33</v>
       </c>
       <c r="E35">
         <f t="shared" si="10"/>
-        <v>56.180339887498945</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="13">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B36">
         <f t="shared" si="8"/>
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="D36">
         <f t="shared" si="9"/>
-        <v>36.617387872822839</v>
+        <v>35.277568135664545</v>
       </c>
       <c r="E36">
         <f t="shared" si="10"/>
-        <v>64.86289650954788</v>
+        <v>58.5</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="13">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B37">
         <f t="shared" si="8"/>
-        <v>348</v>
+        <v>330</v>
       </c>
       <c r="D37">
         <f t="shared" si="9"/>
-        <v>45.8417661836448</v>
+        <v>41.499999999999993</v>
       </c>
       <c r="E37">
         <f t="shared" si="10"/>
-        <v>69.562952014676114</v>
+        <v>64.722431864335448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>